<commit_message>
Transpose Matrix udah bisa
Transpose matrix udah bisa, tinggal Matrix A
</commit_message>
<xml_diff>
--- a/TubesSisrek/pcaProcess/MeanImage.xlsx
+++ b/TubesSisrek/pcaProcess/MeanImage.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -106,7 +106,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -141,7 +141,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>

</xml_diff>